<commit_message>
New visual studio commit
</commit_message>
<xml_diff>
--- a/Список дел.xlsx
+++ b/Список дел.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kotof\OneDrive\Рабочий стол\MyFinance\MyFinance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9551b09a99b3d5f0/Рабочий стол/MyFinance/MyFinance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E55431-78BE-4336-A388-0EE27BDFBA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{F9E55431-78BE-4336-A388-0EE27BDFBA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DDCAB07-B302-4AE8-94A5-3DCF6AC9A3CC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>Работа</t>
   </si>
@@ -288,9 +288,6 @@
     <t>Заказать балкон после 11 апреля</t>
   </si>
   <si>
-    <t>Приготовить материал для игры</t>
-  </si>
-  <si>
     <t>За выходные</t>
   </si>
   <si>
@@ -316,6 +313,24 @@
   </si>
   <si>
     <t>Фауст - 1900</t>
+  </si>
+  <si>
+    <t>В озон</t>
+  </si>
+  <si>
+    <t>Выправить кепку</t>
+  </si>
+  <si>
+    <t>Ждать звонка по стеклу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Домой </t>
+  </si>
+  <si>
+    <t>В кальянку</t>
+  </si>
+  <si>
+    <t>На треню</t>
   </si>
 </sst>
 </file>
@@ -417,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -442,6 +457,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -725,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +789,7 @@
         <v>75</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -794,13 +812,16 @@
         <v>42</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>94</v>
+      <c r="J2" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -826,10 +847,13 @@
         <v>63</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -857,8 +881,11 @@
       <c r="I4" s="6" t="s">
         <v>69</v>
       </c>
+      <c r="J4" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="K4" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -880,8 +907,11 @@
       <c r="H5" s="7" t="s">
         <v>80</v>
       </c>
+      <c r="J5" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="K5" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -901,7 +931,9 @@
         <v>46</v>
       </c>
       <c r="I6"/>
-      <c r="K6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
@@ -919,9 +951,7 @@
       <c r="G7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
@@ -939,7 +969,6 @@
       <c r="G8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
@@ -951,6 +980,9 @@
       <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="F9" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="G9" s="6" t="s">
         <v>49</v>
       </c>
@@ -1045,7 +1077,7 @@
     </row>
     <row r="18" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>57</v>
@@ -1053,7 +1085,7 @@
     </row>
     <row r="19" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>59</v>
@@ -1061,19 +1093,19 @@
     </row>
     <row r="20" spans="2:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22"/>
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>